<commit_message>
Active and Historic Project
</commit_message>
<xml_diff>
--- a/Attachments/dataOne.xlsx
+++ b/Attachments/dataOne.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C3E473-35AA-4B60-8FA2-6CC067C02FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CB4BAB-EB05-493A-A274-9AA32F25A5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE0B157A-249B-4C1C-9000-6E73D773DE83}"/>
   </bookViews>
@@ -751,7 +751,7 @@
   <dimension ref="A1:O202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +870,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="2">
-        <v>2323</v>
+        <v>20026</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Historic and Active Projects
</commit_message>
<xml_diff>
--- a/Attachments/dataOne.xlsx
+++ b/Attachments/dataOne.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CB4BAB-EB05-493A-A274-9AA32F25A5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DD6DB4-5BEE-4B65-8843-7A27D1BA6A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE0B157A-249B-4C1C-9000-6E73D773DE83}"/>
   </bookViews>
@@ -751,7 +751,7 @@
   <dimension ref="A1:O202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +823,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2">
-        <v>2002</v>
+        <v>20031</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>16</v>
@@ -870,7 +870,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="2">
-        <v>20026</v>
+        <v>20032</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>25</v>
@@ -915,7 +915,7 @@
         <v>24</v>
       </c>
       <c r="B4" s="2">
-        <v>3434</v>
+        <v>20033</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>33</v>
@@ -960,7 +960,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="2">
-        <v>4545</v>
+        <v>20034</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>37</v>

</xml_diff>